<commit_message>
Final updates before printing!
</commit_message>
<xml_diff>
--- a/peaks_adjusted.xlsx
+++ b/peaks_adjusted.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="132">
   <si>
     <t>Mount Constance</t>
   </si>
@@ -414,6 +414,15 @@
   </si>
   <si>
     <t>original_y</t>
+  </si>
+  <si>
+    <t>Boston Harbor</t>
+  </si>
+  <si>
+    <t>Pumice Plain</t>
+  </si>
+  <si>
+    <t>Nisqually Wildlife Refuge</t>
   </si>
 </sst>
 </file>
@@ -751,11 +760,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3008,10 +3017,10 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>-123.16891</v>
+        <v>-123.09463700000001</v>
       </c>
       <c r="B85">
-        <v>48.500036999999999</v>
+        <v>48.606878999999999</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>124</v>
@@ -3470,6 +3479,75 @@
       </c>
       <c r="H101" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>-122.903856</v>
+      </c>
+      <c r="B102">
+        <v>47.155270000000002</v>
+      </c>
+      <c r="C102" t="s">
+        <v>129</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E102" t="s">
+        <v>94</v>
+      </c>
+      <c r="F102" s="4">
+        <v>42309</v>
+      </c>
+      <c r="H102" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>-122.173267</v>
+      </c>
+      <c r="B103">
+        <v>46.242195000000002</v>
+      </c>
+      <c r="C103" t="s">
+        <v>130</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E103" t="s">
+        <v>95</v>
+      </c>
+      <c r="F103" s="4">
+        <v>42583</v>
+      </c>
+      <c r="H103" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>-122.694864</v>
+      </c>
+      <c r="B104">
+        <v>47.082683000000003</v>
+      </c>
+      <c r="C104" t="s">
+        <v>131</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E104" t="s">
+        <v>97</v>
+      </c>
+      <c r="F104" s="4">
+        <v>43466</v>
+      </c>
+      <c r="H104" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>